<commit_message>
dodawanie właściwości z deklaracjami i refererencjami + dane testowe
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -71,6 +71,36 @@
   </si>
   <si>
     <t xml:space="preserve">styl malarski obrazu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">followed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">następca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immediately following item in a series of which the subject is a part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">następny element z serii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">follows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poprzednik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immediately prior item in a series of which the subject is a part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poprzedni element z serii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P155</t>
   </si>
   <si>
     <t xml:space="preserve">id_IHPAN</t>
@@ -351,10 +381,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,6 +462,52 @@
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -466,37 +542,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="e">
-        <f aca="false">VLOOKUP(B2, P_list!A2:A6,2, 0)</f>
+        <f aca="false">VLOOKUP(B2, P_list!A2:A7,2, 0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E2" s="0" t="e">
-        <f aca="false">VLOOKUP(D2, P_list!A2:A6,2, 0)</f>
+        <f aca="false">VLOOKUP(D2, P_list!A2:A7,2, 0)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -536,25 +612,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>4</v>
@@ -563,14 +639,14 @@
         <v>5</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <f aca="false">P_list!A4</f>
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="K1" s="0" t="str">
+        <f aca="false">P_list!A5</f>
+        <v>follows</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,31 +654,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1001</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,31 +686,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1002</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="K3" s="2" t="n">
         <f aca="false">C2</f>
@@ -646,13 +722,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>1003</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K4" s="5" t="n">
         <f aca="false">C2</f>
@@ -664,13 +740,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>1004</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,13 +754,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>1005</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,13 +768,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>1006</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,13 +782,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>1007</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,13 +796,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1008</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">C8</f>
@@ -738,13 +814,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>1009</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,13 +828,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1010</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="K11" s="0" t="n">
         <f aca="false">C9</f>

</xml_diff>

<commit_message>
statement: name or id support
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -121,40 +121,52 @@
     <t xml:space="preserve">P155</t>
   </si>
   <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">related properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office of the company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch</t>
+  </si>
+  <si>
     <t xml:space="preserve">id_IHPAN</t>
   </si>
   <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_value_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subclass of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is different</t>
+    <t xml:space="preserve">also_known_as_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also_known_as_pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decription_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiki_url</t>
   </si>
   <si>
     <t xml:space="preserve">instance of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">also_known_as_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">also_known_as_pl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decription_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wiki_url</t>
   </si>
   <si>
     <t xml:space="preserve">geographic object</t>
@@ -260,7 +272,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -289,6 +301,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -360,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -370,6 +396,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,55 +608,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="C2" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="e">
-        <f aca="false">VLOOKUP(B2, P_list!A3:A8,2, 0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="0" t="e">
-        <f aca="false">VLOOKUP(D2, P_list!A3:A8,2, 0)</f>
-        <v>#VALUE!</v>
+      <c r="B4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -661,25 +702,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>4</v>
@@ -688,14 +729,14 @@
         <v>5</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K1" s="0" t="str">
         <f aca="false">P_list!A6</f>
         <v>follows3</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,173 +744,173 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1001</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="n">
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="n">
         <v>1002</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="G3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="5" t="n">
         <f aca="false">C2</f>
         <v>1001</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+    <row r="4" s="8" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="6" t="n">
+      <c r="B4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="8" t="n">
         <v>1003</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="6" t="n">
+      <c r="D4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="8" t="n">
         <f aca="false">C2</f>
         <v>1001</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+    <row r="5" s="8" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="6" t="n">
+      <c r="B5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="8" t="n">
         <v>1004</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="D5" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="6" t="n">
+      <c r="B6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="8" t="n">
         <v>1005</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="D6" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="6" t="n">
+      <c r="B7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8" t="n">
         <v>1006</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="D7" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="7" t="n">
+      <c r="B8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="9" t="n">
         <v>1007</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="D8" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" s="5" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="3" t="n">
+      <c r="B9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="5" t="n">
         <v>1008</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" s="3" t="n">
+      <c r="D9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="5" t="n">
         <f aca="false">C8</f>
         <v>1007</v>
       </c>
     </row>
-    <row r="10" s="7" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" s="9" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="7" t="n">
+      <c r="B10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="9" t="n">
         <v>1009</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>73</v>
+      <c r="D10" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,13 +918,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1010</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K11" s="0" t="n">
         <f aca="false">C9</f>

</xml_diff>

<commit_message>
add update mode, delete test mode
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">styl malarstwa</t>
   </si>
   <si>
-    <t xml:space="preserve">painting style of an object</t>
+    <t xml:space="preserve">EDIT painting style of an object</t>
   </si>
   <si>
     <t xml:space="preserve">styl malarski obrazu</t>
@@ -439,8 +439,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,7 +603,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
support for other data types when adding statements
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -300,7 +300,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -462,10 +462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,7 +475,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,6 +494,7 @@
       <c r="E1" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
imiona, nazwiska - poprawki
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -227,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,6 +256,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -315,7 +321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,6 +335,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,15 +359,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="9:11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.83"/>
@@ -536,6 +546,9 @@
       <c r="F8" s="0" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -556,7 +569,7 @@
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="9:11 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,20 +582,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -690,7 +703,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="9:11 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -705,29 +718,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -750,7 +763,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="9:11 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -760,14 +773,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.49"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
obsługa item cz. 1
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -217,7 +217,52 @@
     <t xml:space="preserve">also_known_as_pl</t>
   </si>
   <si>
-    <t xml:space="preserve">Decription_en</t>
+    <t xml:space="preserve">geographic object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obiekt geograficzny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geographical object | geographic feature | geographic object | topological feature | topological object | topologic feature | topologic object | terrain feature | terrain object | place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obiekt topograficzny | miejsce | obiekt terenowy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">object on a something that can be uniquely identified with geographical data, may be man-made or naturally-created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obiekt, który może być jednoznacznie zidentyfikowany za pomocą danych geograficznych, wytworzony przez człowieka lub w sposób naturalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q618123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jednostka osadnicza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">populated place | settlement | human community | inhabited place | community | human settlements | populated places | settlements | human communities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miejscowość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">community of any size, in which people live</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obszar zamieszkały przez człowieka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q486972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subclass of</t>
   </si>
 </sst>
 </file>
@@ -258,18 +303,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,8 +406,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="9:11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,7 +593,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3"/>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -569,7 +614,7 @@
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="9:11 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -582,20 +627,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>45</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -700,10 +745,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="9:11 B17"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,34 +759,77 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>53</v>
+      <c r="B2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -760,28 +848,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="9:11 C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.32"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>43</v>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsługa dodawania item (strukturalnych/definicyjnych) cd.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="P_statments" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="P_statements" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Q_list" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Q_statments" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Q_statements" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -211,24 +211,12 @@
     <t xml:space="preserve">Nowa_Referencja_01</t>
   </si>
   <si>
-    <t xml:space="preserve">also_known_as_en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">also_known_as_pl</t>
-  </si>
-  <si>
     <t xml:space="preserve">geographic object</t>
   </si>
   <si>
     <t xml:space="preserve">obiekt geograficzny</t>
   </si>
   <si>
-    <t xml:space="preserve">geographical object | geographic feature | geographic object | topological feature | topological object | topologic feature | topologic object | terrain feature | terrain object | place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obiekt topograficzny | miejsce | obiekt terenowy </t>
-  </si>
-  <si>
     <t xml:space="preserve">object on a something that can be uniquely identified with geographical data, may be man-made or naturally-created</t>
   </si>
   <si>
@@ -244,12 +232,6 @@
     <t xml:space="preserve">jednostka osadnicza</t>
   </si>
   <si>
-    <t xml:space="preserve">populated place | settlement | human community | inhabited place | community | human settlements | populated places | settlements | human communities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">miejscowość</t>
-  </si>
-  <si>
     <t xml:space="preserve">community of any size, in which people live</t>
   </si>
   <si>
@@ -263,6 +245,18 @@
   </si>
   <si>
     <t xml:space="preserve">subclass of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obiekt topograficzny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topological object</t>
   </si>
 </sst>
 </file>
@@ -272,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -310,12 +304,6 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -366,7 +354,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,10 +368,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -613,7 +597,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -748,18 +732,17 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,66 +753,50 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +815,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -869,18 +836,40 @@
         <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>71</v>
+      <c r="A2" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
możliwość dodawania 'blokowych' referencji do deklaracji dla właściwości
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -151,6 +151,21 @@
     <t xml:space="preserve">P735</t>
   </si>
   <si>
+    <t xml:space="preserve">my_test_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moja_testowa_właściwość</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testowa właściwość</t>
+  </si>
+  <si>
     <t xml:space="preserve">P</t>
   </si>
   <si>
@@ -202,6 +217,30 @@
     <t xml:space="preserve">ID_SERVICE_201a</t>
   </si>
   <si>
+    <t xml:space="preserve">P148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biurowiec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stated in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122-123</t>
+  </si>
+  <si>
     <t xml:space="preserve">P161</t>
   </si>
   <si>
@@ -299,9 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve">Słownik staropolski, red. S. Urbańczyk, t. 1–11, IJP PAN, Kraków 1953–2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume</t>
   </si>
   <si>
     <t xml:space="preserve">XX</t>
@@ -323,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -360,6 +396,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -411,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,6 +467,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,6 +679,23 @@
         <v>41</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1"/>
     </row>
@@ -652,10 +715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -673,16 +736,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -691,85 +754,119 @@
         <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>59</v>
+      <c r="A7" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -824,70 +921,70 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +1005,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -926,85 +1023,85 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monolingual text, claim value
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">Nowa_Referencja_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pl:To jest tekst w języku polskim</t>
   </si>
   <si>
     <t xml:space="preserve">geographic object</t>
@@ -359,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -396,12 +402,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -453,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -467,10 +467,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,7 +714,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,7 +813,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -864,6 +860,17 @@
       </c>
       <c r="E10" s="0" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -921,70 +928,70 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1026,82 +1033,82 @@
         <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawki do obsługi typów danych
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t xml:space="preserve">pl:”To jest tekst w języku polskim”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+1539-12-08T00:00:00Z/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51.2,20.1</t>
   </si>
   <si>
     <t xml:space="preserve">geographic object</t>
@@ -714,7 +726,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -873,6 +885,29 @@
         <v>76</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -928,70 +963,70 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1033,82 +1068,82 @@
         <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
globalne referencje dla arkuszy z deklaracjami
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="P_statements" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Q_list" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Q_statements" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Global" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Globals" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -371,16 +371,25 @@
     <t xml:space="preserve">administrative division</t>
   </si>
   <si>
+    <t xml:space="preserve">pl:”Tylko test”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sheet</t>
   </si>
   <si>
     <t xml:space="preserve">Q_statements</t>
   </si>
   <si>
-    <t xml:space="preserve">Q79320</t>
+    <t xml:space="preserve">Q79321</t>
   </si>
   <si>
     <t xml:space="preserve">P_statements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ontohgis.pl/</t>
   </si>
 </sst>
 </file>
@@ -527,7 +536,7 @@
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="1" sqref="F:G E10"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -750,8 +759,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="1" sqref="F:G D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -953,7 +962,7 @@
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="F:G A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1070,10 +1079,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="F:G"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1174,6 +1183,17 @@
       </c>
       <c r="C7" s="0" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1195,10 +1215,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="F:G B1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.48"/>
@@ -1207,7 +1227,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1218,21 +1238,30 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://ontohgis.pl/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
deklaracja 'stated as' automatycznie dla aliasów
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -320,15 +320,27 @@
     <t xml:space="preserve">jednostka administracyjna</t>
   </si>
   <si>
-    <t xml:space="preserve">territorial entity for administration purposes, with or without its own local government (v2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jednostka terytorialna wykorzystywana do administracji (w. 2)</t>
+    <t xml:space="preserve">territorial entity for administration purposes, with or without its own local government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jednostka terytorialna wykorzystywana do administracji</t>
   </si>
   <si>
     <t xml:space="preserve">Q56061</t>
   </si>
   <si>
+    <t xml:space="preserve">my_test_item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mój testowy element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My test item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mój element do testów</t>
+  </si>
+  <si>
     <t xml:space="preserve">Value</t>
   </si>
   <si>
@@ -372,6 +384,12 @@
   </si>
   <si>
     <t xml:space="preserve">pl:”Tylko test”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element do testów</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -759,8 +777,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,10 +977,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1061,6 +1079,20 @@
       </c>
       <c r="E5" s="0" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1079,10 +1111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1104,13 +1136,13 @@
         <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1120,7 +1152,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>81</v>
@@ -1132,10 +1164,10 @@
         <v>81</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,10 +1175,10 @@
         <v>81</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,24 +1186,24 @@
         <v>91</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,10 +1211,10 @@
         <v>96</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1225,29 @@
         <v>75</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1272,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.48"/>
@@ -1227,7 +1281,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1238,24 +1292,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodatkowe etykiety i aliasy w językach innych niż en i pl
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="132">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -390,6 +390,18 @@
   </si>
   <si>
     <t xml:space="preserve">Element do testów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das ist ein Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C'est un test</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -1111,10 +1123,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,6 +1260,28 @@
       </c>
       <c r="C10" s="0" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1306,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.48"/>
@@ -1281,7 +1315,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1292,24 +1326,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automatyczne tworzenie deklaracji 'stated as' z aliasów jeżeli istnieje referencja globalna
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -269,6 +269,12 @@
     <t xml:space="preserve">51.2,20.1</t>
   </si>
   <si>
+    <t xml:space="preserve">Described by source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Słownik staropolski, red. S. Urbańczyk, t. 1–11, IJP PAN, Kraków 1953–2002</t>
+  </si>
+  <si>
     <t xml:space="preserve">geographic object</t>
   </si>
   <si>
@@ -365,12 +371,6 @@
     <t xml:space="preserve">topological object</t>
   </si>
   <si>
-    <t xml:space="preserve">Described by source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Słownik staropolski, red. S. Urbańczyk, t. 1–11, IJP PAN, Kraków 1953–2002</t>
-  </si>
-  <si>
     <t xml:space="preserve">XX</t>
   </si>
   <si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t xml:space="preserve">C'est un test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A teraz po włosku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I po hiszpańsku</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -429,7 +441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -466,6 +478,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -525,7 +543,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,6 +561,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +812,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -969,6 +991,17 @@
       </c>
       <c r="C13" s="0" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1027,84 +1060,84 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1123,10 +1156,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,60 +1181,60 @@
         <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>68</v>
@@ -1220,10 +1253,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>118</v>
@@ -1231,7 +1264,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>75</v>
@@ -1242,10 +1275,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>120</v>
@@ -1253,10 +1286,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>121</v>
@@ -1264,7 +1297,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>122</v>
@@ -1275,13 +1308,35 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>124</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1315,35 +1370,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pomijanie istniejących deklaracji i aliasów o takiej samej wartości
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -414,6 +414,15 @@
   </si>
   <si>
     <t xml:space="preserve">I po hiszpańsku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Właściwość pseudonim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drugi pseudonim</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -441,7 +450,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -478,12 +487,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -543,7 +546,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -561,10 +564,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -997,10 +996,10 @@
       <c r="A14" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1156,10 +1155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1189,8 +1188,8 @@
       <c r="E1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1337,6 +1336,39 @@
       </c>
       <c r="C14" s="0" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1370,35 +1402,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pomijanie istniejących deklaracji i aliasów o takiej samej wartości - typy quantity, url
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -425,6 +425,30 @@
     <t xml:space="preserve">Drugi pseudonim</t>
   </si>
   <si>
+    <t xml:space="preserve">P79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://blog.factgrid.de/archives/2833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coordinate location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.33,20.01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sheet</t>
   </si>
   <si>
@@ -435,9 +459,6 @@
   </si>
   <si>
     <t xml:space="preserve">P_statements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reference URL</t>
   </si>
   <si>
     <t xml:space="preserve">https://ontohgis.pl/</t>
@@ -447,8 +468,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -546,7 +568,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,6 +586,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1155,10 +1181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1371,7 +1397,131 @@
         <v>131</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C25" r:id="rId1" display="https://blog.factgrid.de/archives/2833"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1402,7 +1552,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1413,24 +1563,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawki + obsługa dodawania description dla właściwości i elementów
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="154">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -275,6 +275,36 @@
     <t xml:space="preserve">Słownik staropolski, red. S. Urbańczyk, t. 1–11, IJP PAN, Kraków 1953–2002</t>
   </si>
   <si>
+    <t xml:space="preserve">Apl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inna nazwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeszcze inna nazwa po angielsku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etykieta po hiszpańsku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alias po hiszpańsku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis po hiszpańsku</t>
+  </si>
+  <si>
     <t xml:space="preserve">geographic object</t>
   </si>
   <si>
@@ -359,15 +389,9 @@
     <t xml:space="preserve">subclass of</t>
   </si>
   <si>
-    <t xml:space="preserve">Apl</t>
-  </si>
-  <si>
     <t xml:space="preserve">obiekt topograficzny</t>
   </si>
   <si>
-    <t xml:space="preserve">Aen</t>
-  </si>
-  <si>
     <t xml:space="preserve">topological object</t>
   </si>
   <si>
@@ -410,9 +434,6 @@
     <t xml:space="preserve">A teraz po włosku</t>
   </si>
   <si>
-    <t xml:space="preserve">Aes</t>
-  </si>
-  <si>
     <t xml:space="preserve">I po hiszpańsku</t>
   </si>
   <si>
@@ -447,6 +468,9 @@
   </si>
   <si>
     <t xml:space="preserve">50.33,20.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis po hiszpańsku dla elementu</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -837,7 +861,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1027,6 +1051,61 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1085,84 +1164,84 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1181,10 +1260,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1206,54 +1285,54 @@
         <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>81</v>
@@ -1265,144 +1344,144 @@
         <v>68</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>123</v>
@@ -1410,10 +1489,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>100</v>
@@ -1421,10 +1500,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>200</v>
@@ -1432,10 +1511,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>100</v>
@@ -1443,79 +1522,101 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1653,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1563,24 +1664,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>137</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsługa dodatkowej spacji przy monoligualtext
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="154">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -473,19 +473,19 @@
     <t xml:space="preserve">Opis po hiszpańsku dla elementu</t>
   </si>
   <si>
+    <t xml:space="preserve">en: ”Test only”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sheet</t>
   </si>
   <si>
     <t xml:space="preserve">Q_statements</t>
   </si>
   <si>
-    <t xml:space="preserve">Q79321</t>
+    <t xml:space="preserve">https://ontohgis.pl/</t>
   </si>
   <si>
     <t xml:space="preserve">P_statements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ontohgis.pl/</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -541,6 +541,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -592,7 +598,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -614,6 +620,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1260,10 +1270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1617,6 +1627,28 @@
       </c>
       <c r="C30" s="0" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1640,8 +1672,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1653,7 +1685,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1662,31 +1694,32 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>144</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://ontohgis.pl/"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://ontohgis.pl/"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://ontohgis.pl/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
import modelu geo - poprawki
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="159">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -165,6 +165,21 @@
   </si>
   <si>
     <t xml:space="preserve">testowa właściwość (wersja 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purl identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identyfikator purl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external identifier used in OWL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zewnętrzny identyfikator stosowany w OWL</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -496,7 +511,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -520,6 +535,14 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -532,21 +555,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -607,12 +616,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -620,10 +633,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,8 +655,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,106 +672,106 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AMH5" s="0"/>
@@ -849,8 +858,25 @@
         <v>46</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -871,7 +897,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="1:1 A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -884,183 +910,183 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>50</v>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>82</v>
+      <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,10 +1094,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,10 +1105,10 @@
         <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,10 +1116,10 @@
         <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,10 +1127,10 @@
         <v>42</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,10 +1138,10 @@
         <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1139,7 +1165,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="1:1 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1152,20 +1178,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AMH1" s="0"/>
@@ -1173,85 +1199,85 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>97</v>
+      <c r="A2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>102</v>
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1299,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="1" sqref="1:1 C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1287,222 +1313,222 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.61"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="5" t="n">
+        <v>145</v>
+      </c>
+      <c r="C18" s="6" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>100</v>
@@ -1510,10 +1536,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>200</v>
@@ -1521,10 +1547,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>100</v>
@@ -1532,87 +1558,87 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>12</v>
@@ -1620,35 +1646,35 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1672,8 +1698,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="1:1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1684,36 +1710,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>50</v>
+      <c r="A1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsługa dodatkowych kolumn StartsAt, EndsAt, Instance of - początek prac
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -251,6 +251,15 @@
     <t xml:space="preserve">Opis po hiszpańsku</t>
   </si>
   <si>
+    <t xml:space="preserve">StartsAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndsAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instance of</t>
+  </si>
+  <si>
     <t xml:space="preserve">my_test_item</t>
   </si>
   <si>
@@ -263,6 +272,36 @@
     <t xml:space="preserve">Mój element do testów</t>
   </si>
   <si>
+    <t xml:space="preserve">test_item_nr_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test item description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis elementy testowego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q11799456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1525-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q79425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_item_nr_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test item description 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis elementy testowego 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+1532-00-00T00:00:00Z/9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Value</t>
   </si>
   <si>
@@ -330,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">50.33,20.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pl:”Kwalifikator”</t>
   </si>
   <si>
     <t xml:space="preserve">Opis po hiszpańsku dla elementu</t>
@@ -464,7 +506,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -478,6 +520,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -943,17 +989,20 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -973,94 +1022,155 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1531</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1087,8 +1197,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1110,133 +1220,133 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="7" t="n">
+        <v>107</v>
+      </c>
+      <c r="C11" s="8" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -1244,10 +1354,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>200</v>
@@ -1255,10 +1365,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -1266,134 +1376,140 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="D22" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1456,7 +1572,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1469,24 +1585,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nazwy kolumn - poprawki
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="123">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Label_pl</t>
   </si>
   <si>
-    <t xml:space="preserve">datatype</t>
+    <t xml:space="preserve">Datatype</t>
   </si>
   <si>
     <t xml:space="preserve">Description_en</t>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Wiki_id</t>
   </si>
   <si>
-    <t xml:space="preserve">inverse_property</t>
+    <t xml:space="preserve">Inverse_property</t>
   </si>
   <si>
     <t xml:space="preserve">architectural style</t>
@@ -122,13 +122,13 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reference_property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reference_value</t>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference_property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference_value</t>
   </si>
   <si>
     <t xml:space="preserve">related properties</t>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t xml:space="preserve">+1532-00-00T00:00:00Z/9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
   </si>
   <si>
     <t xml:space="preserve">Qualifier</t>
@@ -563,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,8 +986,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1197,8 +1194,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1220,13 +1217,13 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1239,7 +1236,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,7 +1247,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,10 +1255,10 @@
         <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,10 +1266,10 @@
         <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,10 +1277,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,7 +1291,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,10 +1299,10 @@
         <v>78</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,10 +1310,10 @@
         <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,10 +1321,10 @@
         <v>78</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,7 +1332,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>123</v>
@@ -1346,7 +1343,7 @@
         <v>78</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -1357,7 +1354,7 @@
         <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>200</v>
@@ -1368,7 +1365,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -1379,10 +1376,10 @@
         <v>78</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,10 +1387,10 @@
         <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,10 +1398,10 @@
         <v>78</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,10 +1409,10 @@
         <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,10 +1420,10 @@
         <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,10 +1431,10 @@
         <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,10 +1442,10 @@
         <v>78</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1456,7 +1453,7 @@
         <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>12</v>
@@ -1465,7 +1462,7 @@
         <v>59</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1473,7 @@
         <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,7 +1484,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,7 +1495,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1506,10 +1503,10 @@
         <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1573,7 +1570,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1585,7 +1582,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>33</v>
@@ -1596,13 +1593,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wyszukiwanie na podstawie purl
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -272,6 +272,9 @@
     <t xml:space="preserve">Mój element do testów</t>
   </si>
   <si>
+    <t xml:space="preserve">human</t>
+  </si>
+  <si>
     <t xml:space="preserve">test_item_nr_2</t>
   </si>
   <si>
@@ -300,6 +303,18 @@
   </si>
   <si>
     <t xml:space="preserve">+1532-00-00T00:00:00Z/9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_item_nr_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test item description 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opis elementy testowego 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.org/ontohgis#object_95</t>
   </si>
   <si>
     <t xml:space="preserve">Qualifier</t>
@@ -399,9 +414,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -503,7 +519,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,6 +537,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,7 +748,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -986,8 +1006,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1045,129 +1065,164 @@
       <c r="D2" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>1541</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1572</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>1531</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>87</v>
+      <c r="F5" s="0" t="n">
+        <v>1560</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>-120863</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1177,6 +1232,9 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" location="object_95" display="http://purl.org/ontohgis#object_95"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1220,13 +1278,13 @@
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -1236,7 +1294,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1305,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,10 +1313,10 @@
         <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,10 +1324,10 @@
         <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,10 +1335,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,7 +1349,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,10 +1357,10 @@
         <v>78</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,10 +1368,10 @@
         <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,10 +1379,10 @@
         <v>78</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,9 +1390,9 @@
         <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="C11" s="9" t="n">
         <v>123</v>
       </c>
     </row>
@@ -1343,7 +1401,7 @@
         <v>78</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -1354,7 +1412,7 @@
         <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>200</v>
@@ -1365,7 +1423,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -1376,10 +1434,10 @@
         <v>78</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,10 +1445,10 @@
         <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,10 +1456,10 @@
         <v>78</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,10 +1467,10 @@
         <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,10 +1478,10 @@
         <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,10 +1489,10 @@
         <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,10 +1500,10 @@
         <v>78</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1511,7 @@
         <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>12</v>
@@ -1462,7 +1520,7 @@
         <v>59</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,7 +1531,7 @@
         <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1542,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,7 +1553,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,10 +1561,10 @@
         <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1582,24 +1640,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawki do wyszukiwania elementów przez purl
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">Opis elementy testowego 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1569-01-21</t>
   </si>
   <si>
     <t xml:space="preserve">http://purl.org/ontohgis#object_95</t>
@@ -414,10 +417,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -540,8 +542,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -580,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1007,7 +1009,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1146,11 +1148,11 @@
       <c r="F5" s="0" t="n">
         <v>1560</v>
       </c>
-      <c r="G5" s="5" t="n">
-        <v>-120863</v>
+      <c r="G5" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,10 +1280,10 @@
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1294,7 +1296,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1307,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,10 +1315,10 @@
         <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,10 +1326,10 @@
         <v>78</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,10 +1337,10 @@
         <v>78</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1349,7 +1351,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,10 +1359,10 @@
         <v>78</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,10 +1370,10 @@
         <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,10 +1381,10 @@
         <v>78</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,7 +1392,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>123</v>
@@ -1401,7 +1403,7 @@
         <v>78</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -1412,7 +1414,7 @@
         <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>200</v>
@@ -1423,7 +1425,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -1434,10 +1436,10 @@
         <v>78</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,10 +1447,10 @@
         <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1456,10 +1458,10 @@
         <v>78</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,10 +1469,10 @@
         <v>78</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,10 +1480,10 @@
         <v>78</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,10 +1491,10 @@
         <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,10 +1502,10 @@
         <v>78</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1513,7 @@
         <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>12</v>
@@ -1520,7 +1522,7 @@
         <v>59</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,7 +1533,7 @@
         <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1544,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,7 +1555,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,10 +1563,10 @@
         <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1640,7 +1642,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>33</v>
@@ -1651,13 +1653,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsługa somevalue i novalue, język hebrajski w etykietach, opisach i aliasach
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="P_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="134">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -402,6 +402,21 @@
   </si>
   <si>
     <t xml:space="preserve">jeszcze po portugalsku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somevalue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pl:”Redaktor odpowiedzialny”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format publikacji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -514,7 +529,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,6 +568,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1238,8 +1257,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1551,6 +1570,34 @@
       </c>
       <c r="C26" s="0" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1613,7 +1660,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1626,7 +1673,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>33</v>
@@ -1637,13 +1684,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawki, test czytania danych geo
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="137">
   <si>
     <t xml:space="preserve">Label_en</t>
   </si>
@@ -387,6 +387,15 @@
   </si>
   <si>
     <t xml:space="preserve">pl:”Kwalifikator”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de:”Qualifier”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-15</t>
   </si>
   <si>
     <t xml:space="preserve">Opis po hiszpańsku dla elementu</t>
@@ -1257,8 +1266,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1529,25 +1538,19 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>122</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,10 +1558,10 @@
         <v>78</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,42 +1569,62 @@
         <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E29" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1673,7 +1696,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>33</v>
@@ -1684,13 +1707,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>